<commit_message>
added test cases updated username in excel file
</commit_message>
<xml_diff>
--- a/data/Login.xlsx
+++ b/data/Login.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Downloads\Hybrid_Framework-master\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MohanBalakrishnan\Downloads\Docker_Session\webdriver-test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A3C43B-8261-4F5A-8E5A-B6A0FFD9C24D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,13 +36,13 @@
     <t>crmsfa</t>
   </si>
   <si>
-    <t>DemoCSR</t>
+    <t>DemoSalesManager</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -378,11 +379,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="153" zoomScaleNormal="153" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -409,7 +410,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="makaia@testleaf.com"/>
+    <hyperlink ref="A2" r:id="rId1" display="makaia@testleaf.com" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>